<commit_message>
template json support General refactors
</commit_message>
<xml_diff>
--- a/src/app/common/templates/input.xlsx
+++ b/src/app/common/templates/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\boxtrix\src\app\common\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C1A0969-4716-497D-9A32-5BA06A5302CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00B179F-1F2E-47F3-A30E-5C5B20114931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A141BFA4-BF10-4D60-9022-61D08DBFC135}"/>
+    <workbookView xWindow="-38025" yWindow="3000" windowWidth="34020" windowHeight="13410" activeTab="1" xr2:uid="{A141BFA4-BF10-4D60-9022-61D08DBFC135}"/>
   </bookViews>
   <sheets>
     <sheet name="stages" sheetId="3" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>height</t>
   </si>
   <si>
-    <t>deep</t>
-  </si>
-  <si>
     <t>details</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>stage</t>
+  </si>
+  <si>
+    <t>depth</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A14C9F-F7F1-4921-A074-E7A934CF8992}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,15 +515,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E6F4FD-B3B8-4329-B30E-1278EEF96ADD}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,18 +567,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -594,12 +594,12 @@
         <v>STAGE1</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -615,12 +615,12 @@
         <v>STAGE1</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -636,12 +636,12 @@
         <v>STAGE1</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -657,12 +657,12 @@
         <v>STAGE1</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -678,12 +678,12 @@
         <v>STAGE1</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -699,12 +699,12 @@
         <v>STAGE1</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -720,12 +720,12 @@
         <v>STAGE1</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -741,7 +741,7 @@
         <v>STAGE1</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -762,12 +762,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>